<commit_message>
Tablas avance a la mitad
</commit_message>
<xml_diff>
--- a/Docs/Tablas Reto 2.xlsx
+++ b/Docs/Tablas Reto 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanse/Downloads/Universidad de los Andes/2º Semestre/Estructuras de datos y algoritmos/Reto 2/Reto2-G13/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7064598-4C97-844E-8108-B799F9DFBCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EAD789-72D1-4540-9133-E87B4D71B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16960" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Reto" sheetId="1" r:id="rId1"/>
@@ -162,15 +162,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -219,23 +225,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -253,7 +262,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,201 +283,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -775,6 +618,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1329,6 +1196,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1875,6 +1766,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4068,6 +3983,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1171.8800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26468.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75546.880000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>193437.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>335437.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>666984.38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1166515.6200000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1559812.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8607,20 +8546,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:I9" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Requerimiento 1 [ms]" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Requerimiento 2 [ms]" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Requerimiento 3 [ms]" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Requerimiento 4 [ms]" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C763B262-B765-584F-934E-AE938AE06767}" name="Requerimiento 5 [ms]" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{11439835-0545-8648-BAB3-4D28A09D5541}" name="Requerimiento 6 [ms]" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{2BA12E51-2D3B-C244-8593-6ECB6F303CE2}" name="Carga de datos (1) [ms]" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Requerimiento 1 [ms]"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Requerimiento 2 [ms]"/>
+    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Requerimiento 3 [ms]"/>
+    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Requerimiento 4 [ms]"/>
+    <tableColumn id="7" xr3:uid="{C763B262-B765-584F-934E-AE938AE06767}" name="Requerimiento 5 [ms]"/>
+    <tableColumn id="8" xr3:uid="{11439835-0545-8648-BAB3-4D28A09D5541}" name="Requerimiento 6 [ms]"/>
+    <tableColumn id="9" xr3:uid="{2BA12E51-2D3B-C244-8593-6ECB6F303CE2}" name="Carga de datos (1) [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8926,8 +8865,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8940,8 +8879,8 @@
     <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="32">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="32">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -8970,124 +8909,188 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>2716</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="C2" s="17">
+        <v>15.62</v>
+      </c>
+      <c r="D2" s="17">
+        <v>31.25</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17">
+        <v>1171.8800000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>0.05</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>12571</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="C3" s="18">
+        <v>15.62</v>
+      </c>
+      <c r="D3" s="18">
+        <v>46.88</v>
+      </c>
+      <c r="E3" s="18">
+        <v>15.62</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18">
+        <v>26468.75</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>0.1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>21664</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="C4" s="17">
+        <v>15.62</v>
+      </c>
+      <c r="D4" s="17">
+        <v>46.88</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17">
+        <v>75546.880000000005</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>0.2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>38213</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="C5" s="18">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18">
+        <v>62.5</v>
+      </c>
+      <c r="E5" s="18">
+        <v>15.62</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18">
+        <v>193437.5</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>0.3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>53767</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="C6" s="17">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
+        <v>62.5</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17">
+        <v>335437.5</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>0.5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>83569</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="C7" s="18">
+        <v>31.25</v>
+      </c>
+      <c r="D7" s="18">
+        <v>62.5</v>
+      </c>
+      <c r="E7" s="18">
+        <v>15.62</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18">
+        <v>666984.38</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>0.8</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>125924</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="C8" s="17">
+        <v>15.62</v>
+      </c>
+      <c r="D8" s="17">
+        <v>78.12</v>
+      </c>
+      <c r="E8" s="17">
+        <v>31.25</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17">
+        <v>1166515.6200000001</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>153373</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="C9" s="19">
+        <v>15.62</v>
+      </c>
+      <c r="D9" s="19">
+        <v>78.12</v>
+      </c>
+      <c r="E9" s="19">
+        <v>15.62</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19">
+        <v>1559812.5</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="46" customHeight="1">
       <c r="A11" s="11" t="s">
@@ -9096,44 +9099,44 @@
       <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="32">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="32">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -9144,42 +9147,42 @@
       <c r="B19" s="16"/>
     </row>
     <row r="20" spans="1:2" ht="32">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="32">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="36" customHeight="1">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="18"/>
+      <c r="B25" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -9199,124 +9202,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6ca5caf3e573104b48cd489fb7ebf238">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8ff97dc266d6a6a16fe4e7cad907b60" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -9533,10 +9418,139 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9559,20 +9573,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Avance Tabla de Datos
</commit_message>
<xml_diff>
--- a/Docs/Tablas Reto 2.xlsx
+++ b/Docs/Tablas Reto 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanse/Downloads/Universidad de los Andes/2º Semestre/Estructuras de datos y algoritmos/Reto 2/Reto2-G13/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/s_rodriguez63_uniandes_edu_co/Documents/Sicua Plus Andes/Sicua Plus Andes/Tercer Semestre/Estructuras Datos y Algoritmos/Retos/Reto #2/Reto2-G13/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EAD789-72D1-4540-9133-E87B4D71B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{64EAD789-72D1-4540-9133-E87B4D71B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6808CF5A-FA77-4A8C-AC4C-30602E85A2FB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16960" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Reto" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Windows 10 Home 64-Bits</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15.62</t>
+  </si>
+  <si>
+    <t>15.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0</t>
   </si>
 </sst>
 </file>
@@ -268,6 +280,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -285,15 +306,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +426,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -983,7 +995,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1561,7 +1573,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2131,7 +2143,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2339,6 +2351,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2680,7 +2716,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2887,6 +2923,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>46.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>343.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1734.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2876.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4390.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6984.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3228,7 +3288,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3435,6 +3495,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>46.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>203.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>265.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>531.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>687.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3776,7 +3860,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8865,21 +8949,21 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="32">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="27.6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -8908,26 +8992,32 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="5">
         <v>2716</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="11">
         <v>15.62</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="11">
         <v>31.25</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="11">
         <v>0</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17">
+      <c r="F2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="11">
+        <v>46.88</v>
+      </c>
+      <c r="H2" s="11">
+        <v>46.88</v>
+      </c>
+      <c r="I2" s="11">
         <v>1171.8800000000001</v>
       </c>
     </row>
@@ -8938,19 +9028,25 @@
       <c r="B3" s="5">
         <v>12571</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="12">
         <v>15.62</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="12">
         <v>46.88</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="12">
         <v>15.62</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18">
+      <c r="F3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="12">
+        <v>343.75</v>
+      </c>
+      <c r="H3" s="12">
+        <v>203.12</v>
+      </c>
+      <c r="I3" s="12">
         <v>26468.75</v>
       </c>
     </row>
@@ -8961,19 +9057,25 @@
       <c r="B4" s="5">
         <v>21664</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="11">
         <v>15.62</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="11">
         <v>46.88</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="11">
         <v>0</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17">
+      <c r="F4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="11">
+        <v>750</v>
+      </c>
+      <c r="H4" s="11">
+        <v>265.62</v>
+      </c>
+      <c r="I4" s="11">
         <v>75546.880000000005</v>
       </c>
     </row>
@@ -8984,19 +9086,25 @@
       <c r="B5" s="5">
         <v>38213</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="12">
         <v>62.5</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="12">
         <v>15.62</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18">
+      <c r="F5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1734.38</v>
+      </c>
+      <c r="H5" s="12">
+        <v>375</v>
+      </c>
+      <c r="I5" s="12">
         <v>193437.5</v>
       </c>
     </row>
@@ -9007,19 +9115,25 @@
       <c r="B6" s="5">
         <v>53767</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="11">
         <v>0</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="11">
         <v>62.5</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="11">
         <v>0</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17">
+      <c r="F6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="11">
+        <v>2876.24</v>
+      </c>
+      <c r="H6" s="11">
+        <v>425.89</v>
+      </c>
+      <c r="I6" s="11">
         <v>335437.5</v>
       </c>
     </row>
@@ -9030,19 +9144,25 @@
       <c r="B7" s="5">
         <v>83569</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="12">
         <v>31.25</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="12">
         <v>62.5</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="12">
         <v>15.62</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18">
+      <c r="F7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="12">
+        <v>4390.62</v>
+      </c>
+      <c r="H7" s="12">
+        <v>531.25</v>
+      </c>
+      <c r="I7" s="12">
         <v>666984.38</v>
       </c>
     </row>
@@ -9053,62 +9173,74 @@
       <c r="B8" s="5">
         <v>125924</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="11">
         <v>15.62</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="11">
         <v>78.12</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="11">
         <v>31.25</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17">
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="11">
+        <v>6984.38</v>
+      </c>
+      <c r="H8" s="11">
+        <v>640.63</v>
+      </c>
+      <c r="I8" s="11">
         <v>1166515.6200000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16">
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="5">
         <v>153373</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="13">
         <v>15.62</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="13">
         <v>78.12</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="13">
         <v>15.62</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19">
+      <c r="F9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13">
+        <v>9000</v>
+      </c>
+      <c r="H9" s="13">
+        <v>687.5</v>
+      </c>
+      <c r="I9" s="13">
         <v>1559812.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="46" customHeight="1">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:9" ht="46.05" customHeight="1">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="32">
+    <row r="14" spans="1:9" ht="28.8">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -9116,7 +9248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16">
+    <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -9124,7 +9256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16">
+    <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
@@ -9132,7 +9264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="32">
+    <row r="17" spans="1:2" ht="43.2">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -9141,12 +9273,12 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="19"/>
     </row>
-    <row r="20" spans="1:2" ht="32">
+    <row r="20" spans="1:2" ht="28.8">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
@@ -9154,7 +9286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16">
+    <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
@@ -9162,7 +9294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16">
+    <row r="22" spans="1:2">
       <c r="A22" s="7" t="s">
         <v>9</v>
       </c>
@@ -9170,7 +9302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="32">
+    <row r="23" spans="1:2" ht="43.2">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -9179,10 +9311,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="36" customHeight="1">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -9202,6 +9334,115 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6ca5caf3e573104b48cd489fb7ebf238">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8ff97dc266d6a6a16fe4e7cad907b60" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -9418,115 +9659,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9537,6 +9669,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9555,23 +9704,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>

</xml_diff>